<commit_message>
Re-run models for different fiber dispersion values
</commit_message>
<xml_diff>
--- a/BME6250-Biomech2/Homework4/hw5prb1.xlsx
+++ b/BME6250-Biomech2/Homework4/hw5prb1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\GitHub\UtahCoursework\BME6250-Biomech2\Homework4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bulbasaur\GitHub\UtahCoursework\BME6250-Biomech2\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5168A2D-4C90-459E-9B0C-650B272FB799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7376C00-F18C-435C-9425-AC031F6B89F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8985" yWindow="3525" windowWidth="28800" windowHeight="15435" xr2:uid="{BDA0EBF7-6A11-48E0-9CFE-F64BCCCAE5EB}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{BDA0EBF7-6A11-48E0-9CFE-F64BCCCAE5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>k=0</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>k=0.3333</t>
+  </si>
+  <si>
+    <t>E1</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF94734-DB30-4FAA-8F8D-6CA68772FCD2}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,986 +457,1024 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>4.8932000000000002</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3.1364700000000001</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>58.471600000000002</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>1.5986899999999999</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0.85205699999999995</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>7.03931E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B4">
+        <v>4.8932000000000002</v>
+      </c>
+      <c r="C4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4">
+        <v>3.1364399999999999</v>
+      </c>
+      <c r="E4">
         <v>0.01</v>
       </c>
-      <c r="B4">
-        <v>9.8471399999999996</v>
-      </c>
-      <c r="C4">
-        <v>1.2434199999999999E-2</v>
-      </c>
-      <c r="D4">
-        <v>7.8841400000000004</v>
-      </c>
-      <c r="E4">
-        <v>2.8000000000000001E-2</v>
-      </c>
       <c r="F4">
-        <v>10.3147</v>
+        <v>58.471600000000002</v>
       </c>
       <c r="G4">
-        <v>1.9767300000000002E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H4">
-        <v>3.2326800000000002</v>
+        <v>1.5986899999999999</v>
       </c>
       <c r="I4">
-        <v>3.8693100000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J4">
-        <v>1.7741899999999999</v>
+        <v>0.85205699999999995</v>
       </c>
       <c r="K4">
-        <v>4.5999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="L4">
-        <v>2.5733099999999998E-2</v>
+        <v>7.03931E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="B5">
-        <v>24.045200000000001</v>
+        <v>9.8471399999999996</v>
       </c>
       <c r="C5">
-        <v>2.83815E-2</v>
+        <v>1.2434199999999999E-2</v>
       </c>
       <c r="D5">
-        <v>18.4057</v>
+        <v>7.8841200000000002</v>
       </c>
       <c r="E5">
-        <v>4.2689600000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="F5">
-        <v>16.117799999999999</v>
+        <v>10.2194</v>
       </c>
       <c r="G5">
-        <v>3.7581200000000002E-2</v>
+        <v>1.9767300000000002E-2</v>
       </c>
       <c r="H5">
-        <v>6.4008500000000002</v>
+        <v>3.2326800000000002</v>
       </c>
       <c r="I5">
-        <v>6.3647499999999996E-2</v>
+        <v>3.8693100000000001E-2</v>
       </c>
       <c r="J5">
-        <v>3.2043699999999999</v>
+        <v>1.7741899999999999</v>
       </c>
       <c r="K5">
-        <v>7.6799999999999993E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="L5">
-        <v>7.7484399999999995E-2</v>
+        <v>2.5733099999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4.5199999999999997E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="B6">
-        <v>46.480899999999998</v>
+        <v>24.045200000000001</v>
       </c>
       <c r="C6">
-        <v>5.1139400000000002E-2</v>
+        <v>2.83815E-2</v>
       </c>
       <c r="D6">
-        <v>34.239400000000003</v>
+        <v>18.4057</v>
       </c>
       <c r="E6">
-        <v>6.4441300000000007E-2</v>
+        <v>4.36145E-2</v>
       </c>
       <c r="F6">
-        <v>25.230699999999999</v>
+        <v>16.492799999999999</v>
       </c>
       <c r="G6">
-        <v>6.1832199999999997E-2</v>
+        <v>3.7581200000000002E-2</v>
       </c>
       <c r="H6">
-        <v>11.114599999999999</v>
+        <v>6.4008500000000002</v>
       </c>
       <c r="I6">
-        <v>9.3611100000000003E-2</v>
+        <v>6.3647499999999996E-2</v>
       </c>
       <c r="J6">
-        <v>5.2395899999999997</v>
+        <v>3.2043699999999999</v>
       </c>
       <c r="K6">
-        <v>0.11144</v>
+        <v>7.6799999999999993E-2</v>
       </c>
       <c r="L6">
-        <v>0.197403</v>
+        <v>7.7484399999999995E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7.2160000000000002E-2</v>
+        <v>4.5199999999999997E-2</v>
       </c>
       <c r="B7">
-        <v>76.691999999999993</v>
+        <v>46.480899999999998</v>
       </c>
       <c r="C7">
-        <v>7.9345700000000005E-2</v>
+        <v>5.1139400000000002E-2</v>
       </c>
       <c r="D7">
-        <v>55.240499999999997</v>
+        <v>34.239400000000003</v>
       </c>
       <c r="E7">
-        <v>9.1842699999999999E-2</v>
+        <v>6.6105999999999998E-2</v>
       </c>
       <c r="F7">
-        <v>37.610999999999997</v>
+        <v>25.953900000000001</v>
       </c>
       <c r="G7">
-        <v>9.1233099999999998E-2</v>
+        <v>6.1832199999999997E-2</v>
       </c>
       <c r="H7">
-        <v>17.471299999999999</v>
+        <v>11.114599999999999</v>
       </c>
       <c r="I7">
-        <v>0.127582</v>
+        <v>9.3611100000000003E-2</v>
       </c>
       <c r="J7">
-        <v>7.9936999999999996</v>
+        <v>5.2395899999999997</v>
       </c>
       <c r="K7">
-        <v>0.14915200000000001</v>
+        <v>0.11144</v>
       </c>
       <c r="L7">
-        <v>0.43287900000000001</v>
+        <v>0.197403</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.103728</v>
+        <v>7.2160000000000002E-2</v>
       </c>
       <c r="B8">
-        <v>114.554</v>
+        <v>76.691999999999993</v>
       </c>
       <c r="C8">
-        <v>0.111911</v>
+        <v>7.9345700000000005E-2</v>
       </c>
       <c r="D8">
-        <v>81.455799999999996</v>
+        <v>55.240499999999997</v>
       </c>
       <c r="E8">
-        <v>0.123764</v>
+        <v>9.4099299999999997E-2</v>
       </c>
       <c r="F8">
-        <v>53.345799999999997</v>
+        <v>38.676400000000001</v>
       </c>
       <c r="G8">
-        <v>0.124754</v>
+        <v>9.1233099999999998E-2</v>
       </c>
       <c r="H8">
-        <v>25.613600000000002</v>
+        <v>17.471299999999999</v>
       </c>
       <c r="I8">
-        <v>0.16475899999999999</v>
+        <v>0.127582</v>
       </c>
       <c r="J8">
-        <v>11.589</v>
+        <v>7.9936999999999996</v>
       </c>
       <c r="K8">
-        <v>0.18932199999999999</v>
+        <v>0.14915200000000001</v>
       </c>
       <c r="L8">
-        <v>0.840974</v>
+        <v>0.43287900000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.13898199999999999</v>
+        <v>0.103728</v>
       </c>
       <c r="B9">
-        <v>160.16499999999999</v>
+        <v>114.554</v>
       </c>
       <c r="C9">
-        <v>0.14796300000000001</v>
+        <v>0.111911</v>
       </c>
       <c r="D9">
-        <v>113.051</v>
+        <v>81.455799999999996</v>
       </c>
       <c r="E9">
-        <v>0.159301</v>
+        <v>0.126494</v>
       </c>
       <c r="F9">
-        <v>72.594800000000006</v>
+        <v>54.758899999999997</v>
       </c>
       <c r="G9">
-        <v>0.16156999999999999</v>
+        <v>0.124754</v>
       </c>
       <c r="H9">
-        <v>35.707799999999999</v>
+        <v>25.613600000000002</v>
       </c>
       <c r="I9">
-        <v>0.20449999999999999</v>
+        <v>0.16475899999999999</v>
       </c>
       <c r="J9">
-        <v>16.151399999999999</v>
+        <v>11.589</v>
       </c>
       <c r="K9">
-        <v>0.231457</v>
+        <v>0.18932199999999999</v>
       </c>
       <c r="L9">
-        <v>1.48563</v>
+        <v>0.840974</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.17718600000000001</v>
+        <v>0.13898199999999999</v>
       </c>
       <c r="B10">
-        <v>213.773</v>
+        <v>160.16499999999999</v>
       </c>
       <c r="C10">
-        <v>0.186804</v>
+        <v>0.14796300000000001</v>
       </c>
       <c r="D10">
-        <v>150.27199999999999</v>
+        <v>113.051</v>
       </c>
       <c r="E10">
-        <v>0.19772999999999999</v>
+        <v>0.16241</v>
       </c>
       <c r="F10">
-        <v>95.561400000000006</v>
+        <v>74.368300000000005</v>
       </c>
       <c r="G10">
-        <v>0.20102400000000001</v>
+        <v>0.16156999999999999</v>
       </c>
       <c r="H10">
-        <v>47.931399999999996</v>
+        <v>35.707799999999999</v>
       </c>
       <c r="I10">
-        <v>0.24629300000000001</v>
+        <v>0.20449999999999999</v>
       </c>
       <c r="J10">
-        <v>21.807400000000001</v>
+        <v>16.151399999999999</v>
       </c>
       <c r="K10">
-        <v>0.27516600000000002</v>
+        <v>0.231457</v>
       </c>
       <c r="L10">
-        <v>2.4351699999999998</v>
+        <v>1.48563</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.217749</v>
+        <v>0.17718600000000001</v>
       </c>
       <c r="B11">
-        <v>275.745</v>
+        <v>213.773</v>
       </c>
       <c r="C11">
-        <v>0.227878</v>
+        <v>0.186804</v>
       </c>
       <c r="D11">
-        <v>193.42</v>
+        <v>150.27199999999999</v>
       </c>
       <c r="E11">
-        <v>0.23847399999999999</v>
+        <v>0.20114199999999999</v>
       </c>
       <c r="F11">
-        <v>122.477</v>
+        <v>97.712100000000007</v>
       </c>
       <c r="G11">
-        <v>0.242586</v>
+        <v>0.20102400000000001</v>
       </c>
       <c r="H11">
-        <v>62.467399999999998</v>
+        <v>47.931399999999996</v>
       </c>
       <c r="I11">
-        <v>0.28972700000000001</v>
+        <v>0.24629300000000001</v>
       </c>
       <c r="J11">
-        <v>28.682600000000001</v>
+        <v>21.807400000000001</v>
       </c>
       <c r="K11">
-        <v>0.320133</v>
+        <v>0.27516600000000002</v>
       </c>
       <c r="L11">
-        <v>3.7598099999999999</v>
+        <v>2.4351699999999998</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.26019900000000001</v>
+        <v>0.217749</v>
       </c>
       <c r="B12">
-        <v>346.54500000000002</v>
+        <v>275.745</v>
       </c>
       <c r="C12">
-        <v>0.27073599999999998</v>
+        <v>0.227878</v>
       </c>
       <c r="D12">
-        <v>242.84299999999999</v>
+        <v>193.42</v>
       </c>
       <c r="E12">
-        <v>0.28106900000000001</v>
+        <v>0.24212800000000001</v>
       </c>
       <c r="F12">
-        <v>153.59200000000001</v>
+        <v>125.02500000000001</v>
       </c>
       <c r="G12">
-        <v>0.28583599999999998</v>
+        <v>0.242586</v>
       </c>
       <c r="H12">
-        <v>79.501099999999994</v>
+        <v>62.467399999999998</v>
       </c>
       <c r="I12">
-        <v>0.33447500000000002</v>
+        <v>0.28972700000000001</v>
       </c>
       <c r="J12">
-        <v>36.901000000000003</v>
+        <v>28.682600000000001</v>
       </c>
       <c r="K12">
-        <v>0.36610599999999999</v>
+        <v>0.320133</v>
       </c>
       <c r="L12">
-        <v>5.5324799999999996</v>
+        <v>3.7602899999999999</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.30415900000000001</v>
+        <v>0.26019900000000001</v>
       </c>
       <c r="B13">
-        <v>426.726</v>
+        <v>346.54500000000002</v>
       </c>
       <c r="C13">
-        <v>0.315023</v>
+        <v>0.27073599999999998</v>
       </c>
       <c r="D13">
-        <v>298.93299999999999</v>
+        <v>242.84299999999999</v>
       </c>
       <c r="E13">
-        <v>0.32514500000000002</v>
+        <v>0.28491699999999998</v>
       </c>
       <c r="F13">
-        <v>189.17699999999999</v>
+        <v>156.559</v>
       </c>
       <c r="G13">
-        <v>0.33043600000000001</v>
+        <v>0.28583599999999998</v>
       </c>
       <c r="H13">
-        <v>99.220299999999995</v>
+        <v>79.501099999999994</v>
       </c>
       <c r="I13">
-        <v>0.38027300000000003</v>
+        <v>0.33447500000000002</v>
       </c>
       <c r="J13">
-        <v>46.585299999999997</v>
+        <v>36.901000000000003</v>
       </c>
       <c r="K13">
-        <v>0.412885</v>
+        <v>0.36610599999999999</v>
       </c>
       <c r="L13">
-        <v>7.8238599999999998</v>
+        <v>5.5326399999999998</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.349327</v>
+        <v>0.30415900000000001</v>
       </c>
       <c r="B14">
-        <v>516.92899999999997</v>
+        <v>426.726</v>
       </c>
       <c r="C14">
-        <v>0.36045300000000002</v>
+        <v>0.315023</v>
       </c>
       <c r="D14">
-        <v>362.12400000000002</v>
+        <v>298.93299999999999</v>
       </c>
       <c r="E14">
-        <v>0.37040499999999998</v>
+        <v>0.329148</v>
       </c>
       <c r="F14">
-        <v>229.517</v>
+        <v>192.58699999999999</v>
       </c>
       <c r="G14">
-        <v>0.37611600000000001</v>
+        <v>0.33043600000000001</v>
       </c>
       <c r="H14">
-        <v>121.815</v>
+        <v>99.220299999999995</v>
       </c>
       <c r="I14">
-        <v>0.42691200000000001</v>
+        <v>0.38027300000000003</v>
       </c>
       <c r="J14">
-        <v>57.8568</v>
+        <v>46.585299999999997</v>
       </c>
       <c r="K14">
-        <v>0.46030799999999999</v>
+        <v>0.412885</v>
       </c>
       <c r="L14">
-        <v>10.705</v>
+        <v>7.8238599999999998</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.39546199999999998</v>
+        <v>0.349327</v>
       </c>
       <c r="B15">
-        <v>617.89099999999996</v>
+        <v>516.92899999999997</v>
       </c>
       <c r="C15">
-        <v>0.40679599999999999</v>
+        <v>0.36045300000000002</v>
       </c>
       <c r="D15">
-        <v>432.89800000000002</v>
+        <v>362.12400000000002</v>
       </c>
       <c r="E15">
-        <v>0.41661399999999998</v>
+        <v>0.374533</v>
       </c>
       <c r="F15">
-        <v>274.91800000000001</v>
+        <v>233.39500000000001</v>
       </c>
       <c r="G15">
-        <v>0.42265999999999998</v>
+        <v>0.37611600000000001</v>
       </c>
       <c r="H15">
-        <v>147.47999999999999</v>
+        <v>121.815</v>
       </c>
       <c r="I15">
-        <v>0.47422199999999998</v>
+        <v>0.42691200000000001</v>
       </c>
       <c r="J15">
-        <v>70.836600000000004</v>
+        <v>57.8568</v>
       </c>
       <c r="K15">
-        <v>0.50824599999999998</v>
+        <v>0.46030799999999999</v>
       </c>
       <c r="L15">
-        <v>14.2463</v>
+        <v>10.705</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.44236999999999999</v>
+        <v>0.39546199999999998</v>
       </c>
       <c r="B16">
-        <v>730.44500000000005</v>
+        <v>617.89099999999996</v>
       </c>
       <c r="C16">
-        <v>0.45387100000000002</v>
+        <v>0.40679599999999999</v>
       </c>
       <c r="D16">
-        <v>511.78699999999998</v>
+        <v>432.89800000000002</v>
       </c>
       <c r="E16">
-        <v>0.46358100000000002</v>
+        <v>0.42084100000000002</v>
       </c>
       <c r="F16">
-        <v>325.70600000000002</v>
+        <v>279.29300000000001</v>
       </c>
       <c r="G16">
-        <v>0.46989599999999998</v>
+        <v>0.42265999999999998</v>
       </c>
       <c r="H16">
-        <v>176.41499999999999</v>
+        <v>147.47999999999999</v>
       </c>
       <c r="I16">
-        <v>0.52207099999999995</v>
+        <v>0.47422199999999998</v>
       </c>
       <c r="J16">
-        <v>85.646000000000001</v>
+        <v>70.836600000000004</v>
       </c>
       <c r="K16">
-        <v>0.55659700000000001</v>
+        <v>0.50824599999999998</v>
       </c>
       <c r="L16">
-        <v>18.517199999999999</v>
+        <v>14.2463</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.489896</v>
+        <v>0.44236999999999999</v>
       </c>
       <c r="B17">
-        <v>855.54</v>
+        <v>730.44500000000005</v>
       </c>
       <c r="C17">
-        <v>0.50153099999999995</v>
+        <v>0.45387100000000002</v>
       </c>
       <c r="D17">
-        <v>599.38</v>
+        <v>511.78699999999998</v>
       </c>
       <c r="E17">
-        <v>0.511154</v>
+        <v>0.467887</v>
       </c>
       <c r="F17">
-        <v>382.23500000000001</v>
+        <v>330.608</v>
       </c>
       <c r="G17">
-        <v>0.51768400000000003</v>
+        <v>0.46989599999999998</v>
       </c>
       <c r="H17">
-        <v>208.827</v>
+        <v>176.41499999999999</v>
       </c>
       <c r="I17">
-        <v>0.57035000000000002</v>
+        <v>0.52207099999999995</v>
       </c>
       <c r="J17">
-        <v>102.408</v>
+        <v>85.646000000000001</v>
       </c>
       <c r="K17">
-        <v>0.60527799999999998</v>
+        <v>0.55659700000000001</v>
       </c>
       <c r="L17">
-        <v>23.586200000000002</v>
+        <v>18.517199999999999</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.53791599999999995</v>
+        <v>0.489896</v>
       </c>
       <c r="B18">
-        <v>994.24400000000003</v>
+        <v>855.54</v>
       </c>
       <c r="C18">
-        <v>0.54965900000000001</v>
+        <v>0.50153099999999995</v>
       </c>
       <c r="D18">
-        <v>696.33</v>
+        <v>599.38</v>
       </c>
       <c r="E18">
-        <v>0.55921299999999996</v>
+        <v>0.51552399999999998</v>
       </c>
       <c r="F18">
-        <v>444.88499999999999</v>
+        <v>387.69600000000003</v>
       </c>
       <c r="G18">
-        <v>0.56591400000000003</v>
+        <v>0.51768400000000003</v>
       </c>
       <c r="H18">
-        <v>244.935</v>
+        <v>208.827</v>
       </c>
       <c r="I18">
-        <v>0.618973</v>
+        <v>0.57035000000000002</v>
       </c>
       <c r="J18">
-        <v>121.246</v>
+        <v>102.408</v>
       </c>
       <c r="K18">
-        <v>0.65422199999999997</v>
+        <v>0.60527799999999998</v>
       </c>
       <c r="L18">
-        <v>29.5214</v>
+        <v>23.586200000000002</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.58633299999999999</v>
+        <v>0.53791599999999995</v>
       </c>
       <c r="B19">
-        <v>1147.76</v>
+        <v>994.24400000000003</v>
       </c>
       <c r="C19">
-        <v>0.59816100000000005</v>
+        <v>0.54965900000000001</v>
       </c>
       <c r="D19">
-        <v>803.36400000000003</v>
+        <v>696.33</v>
       </c>
       <c r="E19">
-        <v>0.60765999999999998</v>
+        <v>0.56363399999999997</v>
       </c>
       <c r="F19">
-        <v>514.07000000000005</v>
+        <v>450.94099999999997</v>
       </c>
       <c r="G19">
-        <v>0.61449900000000002</v>
+        <v>0.56591400000000003</v>
       </c>
       <c r="H19">
-        <v>284.96600000000001</v>
+        <v>244.935</v>
       </c>
       <c r="I19">
-        <v>0.66787099999999999</v>
+        <v>0.618973</v>
       </c>
       <c r="J19">
-        <v>142.28899999999999</v>
+        <v>121.246</v>
       </c>
       <c r="K19">
-        <v>0.70337799999999995</v>
+        <v>0.65422199999999997</v>
       </c>
       <c r="L19">
-        <v>36.390300000000003</v>
+        <v>29.5214</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.63506700000000005</v>
+        <v>0.58633299999999999</v>
       </c>
       <c r="B20">
-        <v>1317.46</v>
+        <v>1147.76</v>
       </c>
       <c r="C20">
-        <v>0.64696299999999995</v>
+        <v>0.59816100000000005</v>
       </c>
       <c r="D20">
-        <v>921.28700000000003</v>
+        <v>803.36400000000003</v>
       </c>
       <c r="E20">
-        <v>0.65641799999999995</v>
+        <v>0.61212100000000003</v>
       </c>
       <c r="F20">
-        <v>590.24199999999996</v>
+        <v>520.76</v>
       </c>
       <c r="G20">
-        <v>0.66336600000000001</v>
+        <v>0.61449900000000002</v>
       </c>
       <c r="H20">
-        <v>329.16399999999999</v>
+        <v>284.96600000000001</v>
       </c>
       <c r="I20">
-        <v>0.71699000000000002</v>
+        <v>0.66787099999999999</v>
       </c>
       <c r="J20">
-        <v>165.66800000000001</v>
+        <v>142.28899999999999</v>
       </c>
       <c r="K20">
-        <v>0.75270199999999998</v>
+        <v>0.70337799999999995</v>
       </c>
       <c r="L20">
-        <v>44.2607</v>
+        <v>36.390300000000003</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.68405300000000002</v>
+        <v>0.63506700000000005</v>
       </c>
       <c r="B21">
-        <v>1504.86</v>
+        <v>1317.46</v>
       </c>
       <c r="C21">
-        <v>0.69600499999999998</v>
+        <v>0.64696299999999995</v>
       </c>
       <c r="D21">
-        <v>1051</v>
+        <v>921.28700000000003</v>
       </c>
       <c r="E21">
-        <v>0.70542400000000005</v>
+        <v>0.66091200000000005</v>
       </c>
       <c r="F21">
-        <v>673.89300000000003</v>
+        <v>597.60900000000004</v>
       </c>
       <c r="G21">
-        <v>0.71245999999999998</v>
+        <v>0.66336600000000001</v>
       </c>
       <c r="H21">
-        <v>377.78800000000001</v>
+        <v>329.16399999999999</v>
       </c>
       <c r="I21">
-        <v>0.76628499999999999</v>
+        <v>0.71699000000000002</v>
       </c>
       <c r="J21">
-        <v>191.52</v>
+        <v>165.66800000000001</v>
       </c>
       <c r="K21">
-        <v>0.80216200000000004</v>
+        <v>0.75270199999999998</v>
       </c>
       <c r="L21">
-        <v>53.200299999999999</v>
+        <v>44.2607</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.73324299999999998</v>
+        <v>0.68405300000000002</v>
       </c>
       <c r="B22">
-        <v>1711.68</v>
+        <v>1504.86</v>
       </c>
       <c r="C22">
-        <v>0.74523799999999996</v>
+        <v>0.69600499999999998</v>
       </c>
       <c r="D22">
-        <v>1193.49</v>
+        <v>1051</v>
       </c>
       <c r="E22">
-        <v>0.75462899999999999</v>
+        <v>0.70994400000000002</v>
       </c>
       <c r="F22">
-        <v>765.56500000000005</v>
+        <v>681.98500000000001</v>
       </c>
       <c r="G22">
-        <v>0.76173599999999997</v>
+        <v>0.71245999999999998</v>
       </c>
       <c r="H22">
-        <v>431.11399999999998</v>
+        <v>377.78800000000001</v>
       </c>
       <c r="I22">
-        <v>0.81572100000000003</v>
+        <v>0.76628499999999999</v>
       </c>
       <c r="J22">
-        <v>219.98699999999999</v>
+        <v>191.52</v>
       </c>
       <c r="K22">
-        <v>0.85172899999999996</v>
+        <v>0.80216200000000004</v>
       </c>
       <c r="L22">
-        <v>63.2776</v>
+        <v>53.200299999999999</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.78259400000000001</v>
+        <v>0.73323799999999995</v>
       </c>
       <c r="B23">
-        <v>1939.87</v>
+        <v>1711.66</v>
       </c>
       <c r="C23">
-        <v>0.79462500000000003</v>
+        <v>0.74523799999999996</v>
       </c>
       <c r="D23">
-        <v>1349.88</v>
+        <v>1193.49</v>
       </c>
       <c r="E23">
-        <v>0.80399299999999996</v>
+        <v>0.75916899999999998</v>
       </c>
       <c r="F23">
-        <v>865.85</v>
+        <v>774.43299999999999</v>
       </c>
       <c r="G23">
-        <v>0.81115599999999999</v>
+        <v>0.76173599999999997</v>
       </c>
       <c r="H23">
-        <v>489.44</v>
+        <v>431.11399999999998</v>
       </c>
       <c r="I23">
-        <v>0.86526999999999998</v>
+        <v>0.81572100000000003</v>
       </c>
       <c r="J23">
-        <v>251.21700000000001</v>
+        <v>219.98699999999999</v>
       </c>
       <c r="K23">
-        <v>0.90138399999999996</v>
+        <v>0.85172899999999996</v>
       </c>
       <c r="L23">
-        <v>74.561700000000002</v>
+        <v>63.2776</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.83207500000000001</v>
+        <v>0.78258499999999998</v>
       </c>
       <c r="B24">
-        <v>2191.6</v>
+        <v>1939.83</v>
       </c>
       <c r="C24">
-        <v>0.84413400000000005</v>
+        <v>0.79462500000000003</v>
       </c>
       <c r="D24">
-        <v>1521.39</v>
+        <v>1349.88</v>
       </c>
       <c r="E24">
-        <v>0.85348400000000002</v>
+        <v>0.80854999999999999</v>
       </c>
       <c r="F24">
-        <v>975.40099999999995</v>
+        <v>875.55100000000004</v>
       </c>
       <c r="G24">
-        <v>0.86069200000000001</v>
+        <v>0.81115599999999999</v>
       </c>
       <c r="H24">
-        <v>553.08699999999999</v>
+        <v>489.44</v>
       </c>
       <c r="I24">
-        <v>0.91490899999999997</v>
+        <v>0.86526999999999998</v>
       </c>
       <c r="J24">
-        <v>285.36900000000003</v>
+        <v>251.21700000000001</v>
       </c>
       <c r="K24">
-        <v>0.95110700000000004</v>
+        <v>0.90138399999999996</v>
       </c>
       <c r="L24">
-        <v>87.123000000000005</v>
+        <v>74.561700000000002</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0.88166</v>
+        <v>0.832063</v>
       </c>
       <c r="B25">
-        <v>2469.3000000000002</v>
+        <v>2191.54</v>
       </c>
       <c r="C25">
-        <v>0.89374100000000001</v>
+        <v>0.84413400000000005</v>
       </c>
       <c r="D25">
-        <v>1709.41</v>
+        <v>1521.39</v>
       </c>
       <c r="E25">
-        <v>0.90307700000000002</v>
+        <v>0.85805399999999998</v>
       </c>
       <c r="F25">
-        <v>1094.93</v>
+        <v>985.99800000000005</v>
       </c>
       <c r="G25">
-        <v>0.91032100000000005</v>
+        <v>0.86069200000000001</v>
       </c>
       <c r="H25">
-        <v>622.4</v>
+        <v>553.08699999999999</v>
       </c>
       <c r="I25">
-        <v>0.96462000000000003</v>
+        <v>0.91490899999999997</v>
       </c>
       <c r="J25">
-        <v>322.60599999999999</v>
+        <v>285.36900000000003</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>0.95110700000000004</v>
       </c>
       <c r="L25">
-        <v>100.774</v>
+        <v>87.123000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.93132800000000004</v>
+        <v>0.88164600000000004</v>
       </c>
       <c r="B26">
-        <v>2775.7</v>
+        <v>2469.21</v>
       </c>
       <c r="C26">
-        <v>0.94342700000000002</v>
+        <v>0.89374100000000001</v>
       </c>
       <c r="D26">
-        <v>1915.46</v>
+        <v>1709.41</v>
       </c>
       <c r="E26">
-        <v>0.95275100000000001</v>
+        <v>0.90765799999999996</v>
       </c>
       <c r="F26">
-        <v>1225.24</v>
+        <v>1106.5</v>
       </c>
       <c r="G26">
-        <v>0.96002399999999999</v>
+        <v>0.91032100000000005</v>
       </c>
       <c r="H26">
-        <v>697.755</v>
+        <v>622.4</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0.96462000000000003</v>
       </c>
       <c r="J26">
-        <v>351.053</v>
+        <v>322.60599999999999</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>100.774</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.98106300000000002</v>
+        <v>0.93131200000000003</v>
       </c>
       <c r="B27">
-        <v>3113.85</v>
+        <v>2775.59</v>
       </c>
       <c r="C27">
-        <v>0.99317599999999995</v>
+        <v>0.94342700000000002</v>
       </c>
       <c r="D27">
-        <v>2141.2399999999998</v>
+        <v>1915.46</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.957341</v>
       </c>
       <c r="F27">
-        <v>1359.78</v>
+        <v>1237.8399999999999</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0.96002399999999999</v>
       </c>
       <c r="H27">
-        <v>762.94600000000003</v>
+        <v>697.755</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>351.053</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1</v>
+        <v>0.98104499999999994</v>
       </c>
       <c r="B28">
+        <v>3113.73</v>
+      </c>
+      <c r="C28">
+        <v>0.99317599999999995</v>
+      </c>
+      <c r="D28">
+        <v>2141.2399999999998</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1359.78</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>762.94600000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
         <v>3251.55</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
         <v>2173.83</v>
       </c>
     </row>

</xml_diff>